<commit_message>
Windows 10 IoT project started
GPIO Done
I2C ADC in progress
ToDo:
- BLE
 - Temperatures
 - Light
- Benchmark
</commit_message>
<xml_diff>
--- a/Documents/Jegyzetek/Figures/System_design/cable_pinout.xlsx
+++ b/Documents/Jegyzetek/Figures/System_design/cable_pinout.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="51">
   <si>
     <t>GND</t>
   </si>
@@ -122,13 +122,61 @@
     <t>BLE_RST</t>
   </si>
   <si>
-    <t>PE5</t>
-  </si>
-  <si>
     <t>PE4</t>
   </si>
   <si>
     <t>STM32F4</t>
+  </si>
+  <si>
+    <t>PB7</t>
+  </si>
+  <si>
+    <t>PB6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     </t>
+  </si>
+  <si>
+    <t>RaspberryPi</t>
+  </si>
+  <si>
+    <t>GPIO4(7)</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>GPIO17(11)</t>
+  </si>
+  <si>
+    <t>GPIO27(13)</t>
+  </si>
+  <si>
+    <t>GPIO5(29)</t>
+  </si>
+  <si>
+    <t>GPIO6(31)</t>
+  </si>
+  <si>
+    <t>GPIO13(33)</t>
+  </si>
+  <si>
+    <t>UART0RX(8)</t>
+  </si>
+  <si>
+    <t>UART0TX(10)</t>
+  </si>
+  <si>
+    <t>I2C1SCL(5)</t>
+  </si>
+  <si>
+    <t>I2C1SDA(3)</t>
+  </si>
+  <si>
+    <t>GPIO22(15)</t>
+  </si>
+  <si>
+    <t>GPIO18(12)</t>
   </si>
 </sst>
 </file>
@@ -272,9 +320,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -285,6 +330,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -579,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:U15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,103 +641,185 @@
     <col min="5" max="6" width="3.140625" customWidth="1"/>
     <col min="7" max="7" width="16.42578125" customWidth="1"/>
     <col min="8" max="8" width="8.5703125" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" customWidth="1"/>
+    <col min="16" max="16" width="1.42578125" customWidth="1"/>
+    <col min="17" max="18" width="3.140625" customWidth="1"/>
+    <col min="19" max="19" width="16.42578125" customWidth="1"/>
+    <col min="20" max="20" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-    </row>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="M1" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+    </row>
+    <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5"/>
+      <c r="C3" s="4"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="10"/>
+      <c r="G3" s="9"/>
       <c r="H3" t="s">
         <v>22</v>
       </c>
       <c r="I3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M3" t="s">
+        <v>0</v>
+      </c>
+      <c r="N3" t="s">
+        <v>0</v>
+      </c>
+      <c r="O3" s="4"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="9"/>
+      <c r="T3" t="s">
+        <v>38</v>
+      </c>
+      <c r="U3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="5"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="11"/>
+      <c r="G4" s="10"/>
       <c r="H4" t="s">
         <v>23</v>
       </c>
       <c r="I4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M4" t="s">
+        <v>0</v>
+      </c>
+      <c r="N4" t="s">
+        <v>0</v>
+      </c>
+      <c r="O4" s="5"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="10"/>
+      <c r="T4" t="s">
+        <v>39</v>
+      </c>
+      <c r="U4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="6"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="12"/>
+      <c r="G5" s="11"/>
       <c r="H5" t="s">
         <v>24</v>
       </c>
       <c r="I5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N5" t="s">
+        <v>1</v>
+      </c>
+      <c r="O5" s="6"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="11"/>
+      <c r="T5" t="s">
+        <v>39</v>
+      </c>
+      <c r="U5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="8"/>
+      <c r="C6" s="7"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="13"/>
+      <c r="G6" s="12"/>
       <c r="H6" t="s">
         <v>25</v>
       </c>
       <c r="I6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M6" t="s">
+        <v>1</v>
+      </c>
+      <c r="N6" t="s">
+        <v>1</v>
+      </c>
+      <c r="O6" s="7"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="12"/>
+      <c r="T6" t="s">
+        <v>39</v>
+      </c>
+      <c r="U6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="4"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="3"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="1"/>
@@ -699,19 +829,36 @@
       <c r="I7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M7" t="s">
+        <v>2</v>
+      </c>
+      <c r="N7" t="s">
+        <v>40</v>
+      </c>
+      <c r="O7" s="8"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="1"/>
+      <c r="T7" t="s">
+        <v>39</v>
+      </c>
+      <c r="U7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="3"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="10"/>
+      <c r="G8" s="9"/>
       <c r="H8" t="s">
         <v>27</v>
       </c>
@@ -719,88 +866,203 @@
         <v>13</v>
       </c>
       <c r="L8" s="2"/>
-    </row>
-    <row r="9" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M8" t="s">
+        <v>3</v>
+      </c>
+      <c r="N8" t="s">
+        <v>41</v>
+      </c>
+      <c r="O8" s="4"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="9"/>
+      <c r="T8" t="s">
+        <v>42</v>
+      </c>
+      <c r="U8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="5"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="11"/>
+      <c r="G9" s="10"/>
       <c r="H9" t="s">
         <v>28</v>
       </c>
       <c r="I9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M9" t="s">
+        <v>4</v>
+      </c>
+      <c r="N9" t="s">
+        <v>43</v>
+      </c>
+      <c r="O9" s="5"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="10"/>
+      <c r="T9" t="s">
+        <v>39</v>
+      </c>
+      <c r="U9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>5</v>
       </c>
       <c r="B10" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="7"/>
+      <c r="C10" s="6"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="12"/>
+      <c r="G10" s="11"/>
       <c r="H10" t="s">
         <v>29</v>
       </c>
       <c r="I10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M10" t="s">
+        <v>5</v>
+      </c>
+      <c r="N10" t="s">
+        <v>44</v>
+      </c>
+      <c r="O10" s="6"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="11"/>
+      <c r="T10" t="s">
+        <v>39</v>
+      </c>
+      <c r="U10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="8"/>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="7"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="13"/>
+      <c r="G11" s="12"/>
+      <c r="H11" t="s">
+        <v>39</v>
+      </c>
       <c r="I11" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M11" t="s">
+        <v>6</v>
+      </c>
+      <c r="N11" t="s">
+        <v>45</v>
+      </c>
+      <c r="O11" s="7"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="12"/>
+      <c r="T11" t="s">
+        <v>47</v>
+      </c>
+      <c r="U11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="9"/>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="8"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="1"/>
+      <c r="H12" t="s">
+        <v>39</v>
+      </c>
       <c r="I12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M12" t="s">
+        <v>7</v>
+      </c>
+      <c r="N12" t="s">
+        <v>46</v>
+      </c>
+      <c r="O12" s="8"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="1"/>
+      <c r="T12" t="s">
+        <v>48</v>
+      </c>
+      <c r="U12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="N13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="H14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="M14" t="s">
+        <v>30</v>
+      </c>
+      <c r="N14" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="T14" t="s">
+        <v>50</v>
+      </c>
+      <c r="U14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:I1"/>
+    <mergeCell ref="M1:U1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>

</xml_diff>